<commit_message>
Fix APD experiments + better matrix completion experiments
</commit_message>
<xml_diff>
--- a/tests/papers/apd/adp_qsdp.xlsx
+++ b/tests/papers/apd/adp_qsdp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>relative</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
   </si>
 </sst>
 </file>
@@ -102,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,21 +391,20 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="12.36328125" customWidth="1"/>
     <col min="7" max="7" width="8.1796875" customWidth="1"/>
     <col min="8" max="8" width="9.453125" customWidth="1"/>
     <col min="9" max="9" width="8.7265625" customWidth="1"/>
     <col min="10" max="10" width="8.453125" customWidth="1"/>
     <col min="11" max="12" width="11.7265625" customWidth="1"/>
-    <col min="13" max="13" width="10.7265625" customWidth="1"/>
-    <col min="14" max="14" width="9.7265625" customWidth="1"/>
+    <col min="13" max="14" width="10.7265625" customWidth="1"/>
     <col min="15" max="15" width="7.1796875" customWidth="1"/>
     <col min="16" max="16" width="8.6328125" customWidth="1"/>
   </cols>
@@ -467,37 +470,37 @@
         <v>-8.5018220610823256</v>
       </c>
       <c r="D2">
-        <v>-8.5020795999755592</v>
+        <v>-8.5018863550303667</v>
       </c>
       <c r="E2">
         <v>-8.5018220945345995</v>
       </c>
       <c r="F2">
-        <v>-8.5018220825323443</v>
+        <v>-8.5018220504532778</v>
       </c>
       <c r="G2">
         <v>26180</v>
       </c>
       <c r="H2">
-        <v>185214</v>
+        <v>5214</v>
       </c>
       <c r="I2">
         <v>6600</v>
       </c>
       <c r="J2">
-        <v>1128</v>
+        <v>1081</v>
       </c>
       <c r="K2">
-        <v>109.8628198</v>
+        <v>117.0451698</v>
       </c>
       <c r="L2">
-        <v>1166.5728552</v>
+        <v>34.481060800000002</v>
       </c>
       <c r="M2">
-        <v>17.304888600000002</v>
+        <v>18.134335799999999</v>
       </c>
       <c r="N2">
-        <v>4.3650393999999997</v>
+        <v>4.3878937999999996</v>
       </c>
       <c r="O2">
         <v>9.9999999999999995E-7</v>
@@ -517,37 +520,37 @@
         <v>-7.6040844172213928</v>
       </c>
       <c r="D3">
-        <v>-7.5401554562188364</v>
+        <v>-7.6059659972623432</v>
       </c>
       <c r="E3">
         <v>-7.6040838414526792</v>
       </c>
       <c r="F3">
-        <v>-7.6040833556685659</v>
+        <v>-7.6040824603427222</v>
       </c>
       <c r="G3">
         <v>75680</v>
       </c>
       <c r="H3">
-        <v>381841</v>
+        <v>11081</v>
       </c>
       <c r="I3">
         <v>6981</v>
       </c>
       <c r="J3">
-        <v>3377</v>
+        <v>3343</v>
       </c>
       <c r="K3">
-        <v>315.92184459999999</v>
+        <v>339.65846820000002</v>
       </c>
       <c r="L3">
-        <v>2400.0064526000001</v>
+        <v>74.6775758</v>
       </c>
       <c r="M3">
-        <v>18.304715999999999</v>
+        <v>19.734525399999999</v>
       </c>
       <c r="N3">
-        <v>12.980953100000001</v>
+        <v>14.318149699999999</v>
       </c>
       <c r="O3">
         <v>9.9999999999999995E-7</v>
@@ -567,37 +570,37 @@
         <v>-7.5118606610455041</v>
       </c>
       <c r="D4">
-        <v>-7.5129640900701133</v>
+        <v>-7.52091268779711</v>
       </c>
       <c r="E4">
         <v>-7.5119343437537482</v>
       </c>
       <c r="F4">
-        <v>-7.5116370576260394</v>
+        <v>-7.5115525143231654</v>
       </c>
       <c r="G4">
         <v>121618</v>
       </c>
       <c r="H4">
-        <v>26633</v>
+        <v>14821</v>
       </c>
       <c r="I4">
         <v>22096</v>
       </c>
       <c r="J4">
-        <v>7228</v>
+        <v>7110</v>
       </c>
       <c r="K4">
-        <v>502.49499049999997</v>
+        <v>557.11907120000001</v>
       </c>
       <c r="L4">
-        <v>166.56637129999999</v>
+        <v>98.619882000000004</v>
       </c>
       <c r="M4">
-        <v>61.3182586</v>
+        <v>60.7317447</v>
       </c>
       <c r="N4">
-        <v>30.869702700000001</v>
+        <v>29.198791199999999</v>
       </c>
       <c r="O4">
         <v>9.9999999999999995E-7</v>
@@ -608,152 +611,152 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
-        <v>9999.9999999878582</v>
+        <v>999.99999998416752</v>
       </c>
       <c r="B5">
-        <v>100000</v>
+        <v>10000000</v>
       </c>
       <c r="C5">
-        <v>-1163.2890440621363</v>
+        <v>-75.118606610455046</v>
       </c>
       <c r="D5">
-        <v>-1163.205625288869</v>
+        <v>-75.211016239359864</v>
       </c>
       <c r="E5">
-        <v>-1163.2890441100908</v>
+        <v>-75.119343437537523</v>
       </c>
       <c r="F5">
-        <v>-1163.2890441095806</v>
+        <v>-75.115852522396793</v>
       </c>
       <c r="G5">
-        <v>3034</v>
+        <v>121618</v>
       </c>
       <c r="H5">
-        <v>383343</v>
+        <v>14825</v>
       </c>
       <c r="I5">
-        <v>1268</v>
+        <v>22096</v>
       </c>
       <c r="J5">
-        <v>943</v>
+        <v>10142</v>
       </c>
       <c r="K5">
-        <v>12.5256089</v>
+        <v>576.85369419999995</v>
       </c>
       <c r="L5">
-        <v>2400.0062868999998</v>
+        <v>106.7051043</v>
       </c>
       <c r="M5">
-        <v>3.2771452999999999</v>
+        <v>63.215575399999999</v>
       </c>
       <c r="N5">
-        <v>3.5644181000000001</v>
+        <v>43.854207600000002</v>
       </c>
       <c r="O5">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="P5" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6">
-        <v>999.99999995174585</v>
-      </c>
-      <c r="B6">
-        <v>100000.00000000001</v>
+        <v>99.999999999170242</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9999999.9990916178</v>
       </c>
       <c r="C6">
-        <v>-85.01822061135185</v>
+        <v>-7.4988601076838552</v>
       </c>
       <c r="D6">
-        <v>-85.021422459843535</v>
+        <v>-5.5992913022744695</v>
       </c>
       <c r="E6">
-        <v>-85.018220945345874</v>
+        <v>-7.5020552480901657</v>
       </c>
       <c r="F6">
-        <v>-85.018220943780918</v>
+        <v>-7.458520253104405</v>
       </c>
       <c r="G6">
-        <v>26184</v>
+        <v>130302</v>
       </c>
       <c r="H6">
-        <v>375106</v>
+        <v>16582</v>
       </c>
       <c r="I6">
-        <v>6600</v>
+        <v>32743</v>
       </c>
       <c r="J6">
-        <v>2173</v>
+        <v>11893</v>
       </c>
       <c r="K6">
-        <v>108.4949422</v>
+        <v>611.52229339999997</v>
       </c>
       <c r="L6">
-        <v>2400.0024321999999</v>
+        <v>114.7723979</v>
       </c>
       <c r="M6">
-        <v>17.708777900000001</v>
+        <v>92.425136199999997</v>
       </c>
       <c r="N6">
-        <v>8.2070709999999991</v>
+        <v>50.775841</v>
       </c>
       <c r="O6">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="P6" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7">
-        <v>100.00000000000544</v>
+        <v>10.000000000698492</v>
       </c>
       <c r="B7">
-        <v>99999.999999942767</v>
+        <v>9999999.9999999963</v>
       </c>
       <c r="C7">
-        <v>-7.6040844172213928</v>
+        <v>-0.74877875924638793</v>
       </c>
       <c r="D7">
-        <v>-7.5647250984233123</v>
+        <v>0.69724256207684965</v>
       </c>
       <c r="E7">
-        <v>-7.6040838414526792</v>
+        <v>-0.71090728929024405</v>
       </c>
       <c r="F7">
-        <v>-7.6040833556685659</v>
+        <v>-0.68106492539102848</v>
       </c>
       <c r="G7">
-        <v>75680</v>
+        <v>230428</v>
       </c>
       <c r="H7">
-        <v>371071</v>
+        <v>35410</v>
       </c>
       <c r="I7">
-        <v>6981</v>
+        <v>26509</v>
       </c>
       <c r="J7">
-        <v>3377</v>
+        <v>20375</v>
       </c>
       <c r="K7">
-        <v>321.24151000000001</v>
+        <v>1074.6186835000001</v>
       </c>
       <c r="L7">
-        <v>2400.0056092999998</v>
+        <v>241.800633</v>
       </c>
       <c r="M7">
-        <v>19.1480268</v>
+        <v>73.434905499999999</v>
       </c>
       <c r="N7">
-        <v>13.569318600000001</v>
+        <v>85.397531200000003</v>
       </c>
       <c r="O7">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="P7" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sparse PCA experiments
</commit_message>
<xml_diff>
--- a/tests/papers/apd/adp_qsdp.xlsx
+++ b/tests/papers/apd/adp_qsdp.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -14,12 +14,114 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_UPF</t>
+  </si>
+  <si>
+    <t>fval_ANCF</t>
+  </si>
+  <si>
+    <t>fval_AIPP</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_UPF</t>
+  </si>
+  <si>
+    <t>iter_ANCF</t>
+  </si>
+  <si>
+    <t>iter_AIPP</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>t_UPF</t>
+  </si>
+  <si>
+    <t>t_ANCF</t>
+  </si>
+  <si>
+    <t>t_AIPP</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_UPF</t>
+  </si>
+  <si>
+    <t>fval_ANCF</t>
+  </si>
+  <si>
+    <t>fval_AIPP</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_UPF</t>
+  </si>
+  <si>
+    <t>iter_ANCF</t>
+  </si>
+  <si>
+    <t>iter_AIPP</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>t_UPF</t>
+  </si>
+  <si>
+    <t>t_ANCF</t>
+  </si>
+  <si>
+    <t>t_AIPP</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
   <si>
     <t>relative</t>
   </si>
@@ -93,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,13 +203,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,276 +496,281 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.36328125" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" customWidth="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1"/>
-    <col min="11" max="12" width="11.7265625" customWidth="1"/>
-    <col min="13" max="14" width="10.7265625" customWidth="1"/>
-    <col min="15" max="15" width="7.1796875" customWidth="1"/>
-    <col min="16" max="16" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.16796875" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="12.34765625" customWidth="true"/>
+    <col min="7" max="7" width="8.16796875" customWidth="true"/>
+    <col min="8" max="8" width="9.44140625" customWidth="true"/>
+    <col min="9" max="9" width="8.7109375" customWidth="true"/>
+    <col min="10" max="10" width="8.44140625" customWidth="true"/>
+    <col min="11" max="11" width="11.7109375" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="15" max="15" width="7.16796875" customWidth="true"/>
+    <col min="16" max="16" width="8.62109375" customWidth="true"/>
+    <col min="4" max="4" width="12.34765625" customWidth="true"/>
+    <col min="5" max="5" width="12.34765625" customWidth="true"/>
+    <col min="6" max="6" width="12.34765625" customWidth="true"/>
+    <col min="12" max="12" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="10.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2">
-        <v>99.999999995177177</v>
-      </c>
-      <c r="B2">
-        <v>10000.000000000015</v>
-      </c>
-      <c r="C2">
-        <v>-8.5018220610823256</v>
-      </c>
-      <c r="D2">
-        <v>-8.5018863550303667</v>
-      </c>
-      <c r="E2">
-        <v>-8.5018220945345995</v>
-      </c>
-      <c r="F2">
-        <v>-8.5018220504532778</v>
-      </c>
-      <c r="G2">
-        <v>26180</v>
-      </c>
-      <c r="H2">
-        <v>5214</v>
-      </c>
-      <c r="I2">
-        <v>6600</v>
-      </c>
-      <c r="J2">
-        <v>1081</v>
-      </c>
-      <c r="K2">
-        <v>117.0451698</v>
-      </c>
-      <c r="L2">
-        <v>34.481060800000002</v>
-      </c>
-      <c r="M2">
-        <v>18.134335799999999</v>
-      </c>
-      <c r="N2">
-        <v>4.3878937999999996</v>
-      </c>
-      <c r="O2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="P2" t="s">
-        <v>0</v>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>99.999999998151907</v>
+      </c>
+      <c r="B2" s="0">
+        <v>1000000.0000000008</v>
+      </c>
+      <c r="C2" s="0">
+        <v>-7.5118606610455041</v>
+      </c>
+      <c r="D2" s="0">
+        <v>-7.52091268779711</v>
+      </c>
+      <c r="E2" s="0">
+        <v>-7.5101307468924752</v>
+      </c>
+      <c r="F2" s="0">
+        <v>-7.5115525143231654</v>
+      </c>
+      <c r="G2" s="0">
+        <v>121618</v>
+      </c>
+      <c r="H2" s="0">
+        <v>14821</v>
+      </c>
+      <c r="I2" s="0">
+        <v>375600</v>
+      </c>
+      <c r="J2" s="0">
+        <v>7110</v>
+      </c>
+      <c r="K2" s="0">
+        <v>512.31850229999998</v>
+      </c>
+      <c r="L2" s="0">
+        <v>92.134071500000005</v>
+      </c>
+      <c r="M2" s="0">
+        <v>1200.0024409</v>
+      </c>
+      <c r="N2" s="0">
+        <v>28.6171939</v>
+      </c>
+      <c r="O2" s="0">
+        <v>9.9999999999999995e-07</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3">
-        <v>100.00000000000544</v>
-      </c>
-      <c r="B3">
-        <v>99999.999999942767</v>
-      </c>
-      <c r="C3">
-        <v>-7.6040844172213928</v>
-      </c>
-      <c r="D3">
-        <v>-7.6059659972623432</v>
-      </c>
-      <c r="E3">
-        <v>-7.6040838414526792</v>
-      </c>
-      <c r="F3">
-        <v>-7.6040824603427222</v>
-      </c>
-      <c r="G3">
-        <v>75680</v>
-      </c>
-      <c r="H3">
-        <v>11081</v>
-      </c>
-      <c r="I3">
-        <v>6981</v>
-      </c>
-      <c r="J3">
-        <v>3343</v>
-      </c>
-      <c r="K3">
-        <v>339.65846820000002</v>
-      </c>
-      <c r="L3">
-        <v>74.6775758</v>
-      </c>
-      <c r="M3">
-        <v>19.734525399999999</v>
-      </c>
-      <c r="N3">
-        <v>14.318149699999999</v>
-      </c>
-      <c r="O3">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="P3" t="s">
-        <v>0</v>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>999.99999998416752</v>
+      </c>
+      <c r="B3" s="0">
+        <v>10000000</v>
+      </c>
+      <c r="C3" s="0">
+        <v>-75.118606610455046</v>
+      </c>
+      <c r="D3" s="0">
+        <v>-75.211016239359864</v>
+      </c>
+      <c r="E3" s="0">
+        <v>-75.101516152466402</v>
+      </c>
+      <c r="F3" s="0">
+        <v>-75.115852522396793</v>
+      </c>
+      <c r="G3" s="0">
+        <v>121618</v>
+      </c>
+      <c r="H3" s="0">
+        <v>14825</v>
+      </c>
+      <c r="I3" s="0">
+        <v>379446</v>
+      </c>
+      <c r="J3" s="0">
+        <v>10142</v>
+      </c>
+      <c r="K3" s="0">
+        <v>515.77433689999998</v>
+      </c>
+      <c r="L3" s="0">
+        <v>93.661196399999994</v>
+      </c>
+      <c r="M3" s="0">
+        <v>1200.0062187999999</v>
+      </c>
+      <c r="N3" s="0">
+        <v>40.084657900000003</v>
+      </c>
+      <c r="O3" s="0">
+        <v>9.9999999999999995e-07</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4">
-        <v>99.999999998151907</v>
-      </c>
-      <c r="B4">
-        <v>1000000.0000000008</v>
-      </c>
-      <c r="C4">
-        <v>-7.5118606610455041</v>
-      </c>
-      <c r="D4">
-        <v>-7.52091268779711</v>
-      </c>
-      <c r="E4">
-        <v>-7.5119343437537482</v>
-      </c>
-      <c r="F4">
-        <v>-7.5115525143231654</v>
-      </c>
-      <c r="G4">
-        <v>121618</v>
-      </c>
-      <c r="H4">
-        <v>14821</v>
-      </c>
-      <c r="I4">
-        <v>22096</v>
-      </c>
-      <c r="J4">
-        <v>7110</v>
-      </c>
-      <c r="K4">
-        <v>557.11907120000001</v>
-      </c>
-      <c r="L4">
-        <v>98.619882000000004</v>
-      </c>
-      <c r="M4">
-        <v>60.7317447</v>
-      </c>
-      <c r="N4">
-        <v>29.198791199999999</v>
-      </c>
-      <c r="O4">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="P4" t="s">
-        <v>0</v>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>99.999999999170242</v>
+      </c>
+      <c r="B4" s="0">
+        <v>9999999.9990916178</v>
+      </c>
+      <c r="C4" s="0">
+        <v>-7.4988601076838552</v>
+      </c>
+      <c r="D4" s="0">
+        <v>-5.5992913022744695</v>
+      </c>
+      <c r="E4" s="0">
+        <v>-7.456839633913436</v>
+      </c>
+      <c r="F4" s="0">
+        <v>-7.458520253104405</v>
+      </c>
+      <c r="G4" s="0">
+        <v>130302</v>
+      </c>
+      <c r="H4" s="0">
+        <v>16582</v>
+      </c>
+      <c r="I4" s="0">
+        <v>132227</v>
+      </c>
+      <c r="J4" s="0">
+        <v>11893</v>
+      </c>
+      <c r="K4" s="0">
+        <v>550.31302019999998</v>
+      </c>
+      <c r="L4" s="0">
+        <v>104.7295883</v>
+      </c>
+      <c r="M4" s="0">
+        <v>346.84264990000003</v>
+      </c>
+      <c r="N4" s="0">
+        <v>47.024495899999998</v>
+      </c>
+      <c r="O4" s="0">
+        <v>9.9999999999999995e-07</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5">
-        <v>999.99999998416752</v>
-      </c>
-      <c r="B5">
-        <v>10000000</v>
-      </c>
-      <c r="C5">
-        <v>-75.118606610455046</v>
-      </c>
-      <c r="D5">
-        <v>-75.211016239359864</v>
-      </c>
-      <c r="E5">
-        <v>-75.119343437537523</v>
-      </c>
-      <c r="F5">
-        <v>-75.115852522396793</v>
-      </c>
-      <c r="G5">
-        <v>121618</v>
-      </c>
-      <c r="H5">
-        <v>14825</v>
-      </c>
-      <c r="I5">
-        <v>22096</v>
-      </c>
-      <c r="J5">
-        <v>10142</v>
-      </c>
-      <c r="K5">
-        <v>576.85369419999995</v>
-      </c>
-      <c r="L5">
-        <v>106.7051043</v>
-      </c>
-      <c r="M5">
-        <v>63.215575399999999</v>
-      </c>
-      <c r="N5">
-        <v>43.854207600000002</v>
-      </c>
-      <c r="O5">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="P5" t="s">
-        <v>17</v>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>10.000000000698492</v>
+      </c>
+      <c r="B5" s="0">
+        <v>9999999.9999999963</v>
+      </c>
+      <c r="C5" s="0">
+        <v>-0.74877875924638793</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.69724256207684965</v>
+      </c>
+      <c r="E5" s="0">
+        <v>-0.66132844733308338</v>
+      </c>
+      <c r="F5" s="0">
+        <v>-0.68106492539102848</v>
+      </c>
+      <c r="G5" s="0">
+        <v>230428</v>
+      </c>
+      <c r="H5" s="0">
+        <v>35410</v>
+      </c>
+      <c r="I5" s="0">
+        <v>43961</v>
+      </c>
+      <c r="J5" s="0">
+        <v>20375</v>
+      </c>
+      <c r="K5" s="0">
+        <v>994.06765700000005</v>
+      </c>
+      <c r="L5" s="0">
+        <v>225.58642130000001</v>
+      </c>
+      <c r="M5" s="0">
+        <v>116.73129950000001</v>
+      </c>
+      <c r="N5" s="0">
+        <v>81.480997400000007</v>
+      </c>
+      <c r="O5" s="0">
+        <v>9.9999999999999995e-07</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6">
       <c r="A6">
         <v>99.999999999170242</v>
       </c>
@@ -709,7 +820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7">
       <c r="A7">
         <v>10.000000000698492</v>
       </c>

</xml_diff>

<commit_message>
Improvements to the APD experiments
</commit_message>
<xml_diff>
--- a/tests/papers/apd/adp_qsdp.xlsx
+++ b/tests/papers/apd/adp_qsdp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="349">
   <si>
     <t>relative</t>
   </si>
@@ -154,6 +154,897 @@
   </si>
   <si>
     <t>iter_APD</t>
+  </si>
+  <si>
+    <t>t_UPF</t>
+  </si>
+  <si>
+    <t>t_ANCF</t>
+  </si>
+  <si>
+    <t>t_AIPP</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_UPF</t>
+  </si>
+  <si>
+    <t>fval_ANCF</t>
+  </si>
+  <si>
+    <t>fval_AIPP</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_UPF</t>
+  </si>
+  <si>
+    <t>iter_ANCF</t>
+  </si>
+  <si>
+    <t>iter_AIPP</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>t_UPF</t>
+  </si>
+  <si>
+    <t>t_ANCF</t>
+  </si>
+  <si>
+    <t>t_AIPP</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_UPF</t>
+  </si>
+  <si>
+    <t>fval_ANCF</t>
+  </si>
+  <si>
+    <t>fval_AIPP</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_UPF</t>
+  </si>
+  <si>
+    <t>iter_ANCF</t>
+  </si>
+  <si>
+    <t>iter_AIPP</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_UPF</t>
+  </si>
+  <si>
+    <t>fn_iter_ANCF</t>
+  </si>
+  <si>
+    <t>fn_iter_AIPP</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_UPF</t>
+  </si>
+  <si>
+    <t>grad_iter_ANCF</t>
+  </si>
+  <si>
+    <t>grad_iter_AIPP</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_UPF</t>
+  </si>
+  <si>
+    <t>t_ANCF</t>
+  </si>
+  <si>
+    <t>t_AIPP</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_UPF</t>
+  </si>
+  <si>
+    <t>fval_ANCF</t>
+  </si>
+  <si>
+    <t>fval_AIPP</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_UPF</t>
+  </si>
+  <si>
+    <t>iter_ANCF</t>
+  </si>
+  <si>
+    <t>iter_AIPP</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_UPF</t>
+  </si>
+  <si>
+    <t>fn_iter_ANCF</t>
+  </si>
+  <si>
+    <t>fn_iter_AIPP</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_UPF</t>
+  </si>
+  <si>
+    <t>grad_iter_ANCF</t>
+  </si>
+  <si>
+    <t>grad_iter_AIPP</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_UPF</t>
+  </si>
+  <si>
+    <t>t_ANCF</t>
+  </si>
+  <si>
+    <t>t_AIPP</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_UPF</t>
+  </si>
+  <si>
+    <t>fval_ANCF</t>
+  </si>
+  <si>
+    <t>fval_AIPP</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_UPF</t>
+  </si>
+  <si>
+    <t>iter_ANCF</t>
+  </si>
+  <si>
+    <t>iter_AIPP</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_UPF</t>
+  </si>
+  <si>
+    <t>fn_iter_ANCF</t>
+  </si>
+  <si>
+    <t>fn_iter_AIPP</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_UPF</t>
+  </si>
+  <si>
+    <t>grad_iter_ANCF</t>
+  </si>
+  <si>
+    <t>grad_iter_AIPP</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_UPF</t>
+  </si>
+  <si>
+    <t>t_ANCF</t>
+  </si>
+  <si>
+    <t>t_AIPP</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_UPF</t>
+  </si>
+  <si>
+    <t>fval_ANCF</t>
+  </si>
+  <si>
+    <t>fval_AIPP</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_UPF</t>
+  </si>
+  <si>
+    <t>iter_ANCF</t>
+  </si>
+  <si>
+    <t>iter_AIPP</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_UPF</t>
+  </si>
+  <si>
+    <t>fn_iter_ANCF</t>
+  </si>
+  <si>
+    <t>fn_iter_AIPP</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_UPF</t>
+  </si>
+  <si>
+    <t>grad_iter_ANCF</t>
+  </si>
+  <si>
+    <t>grad_iter_AIPP</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_UPF</t>
+  </si>
+  <si>
+    <t>t_ANCF</t>
+  </si>
+  <si>
+    <t>t_AIPP</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_UPF</t>
+  </si>
+  <si>
+    <t>fval_ANCF</t>
+  </si>
+  <si>
+    <t>fval_AIPP</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_UPF</t>
+  </si>
+  <si>
+    <t>iter_ANCF</t>
+  </si>
+  <si>
+    <t>iter_AIPP</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_UPF</t>
+  </si>
+  <si>
+    <t>fn_iter_ANCF</t>
+  </si>
+  <si>
+    <t>fn_iter_AIPP</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_UPF</t>
+  </si>
+  <si>
+    <t>grad_iter_ANCF</t>
+  </si>
+  <si>
+    <t>grad_iter_AIPP</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_UPF</t>
+  </si>
+  <si>
+    <t>t_ANCF</t>
+  </si>
+  <si>
+    <t>t_AIPP</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
+  </si>
+  <si>
+    <t>t_APD</t>
+  </si>
+  <si>
+    <t>opt_tol</t>
+  </si>
+  <si>
+    <t>opt_type</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>fval_UPF</t>
+  </si>
+  <si>
+    <t>fval_ANCF</t>
+  </si>
+  <si>
+    <t>fval_AIPP</t>
+  </si>
+  <si>
+    <t>fval_APD</t>
+  </si>
+  <si>
+    <t>iter_UPF</t>
+  </si>
+  <si>
+    <t>iter_ANCF</t>
+  </si>
+  <si>
+    <t>iter_AIPP</t>
+  </si>
+  <si>
+    <t>iter_APD</t>
+  </si>
+  <si>
+    <t>fn_iter_UPF</t>
+  </si>
+  <si>
+    <t>fn_iter_ANCF</t>
+  </si>
+  <si>
+    <t>fn_iter_AIPP</t>
+  </si>
+  <si>
+    <t>fn_iter_APD</t>
+  </si>
+  <si>
+    <t>grad_iter_UPF</t>
+  </si>
+  <si>
+    <t>grad_iter_ANCF</t>
+  </si>
+  <si>
+    <t>grad_iter_AIPP</t>
+  </si>
+  <si>
+    <t>grad_iter_APD</t>
   </si>
   <si>
     <t>t_UPF</t>
@@ -494,7 +1385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
@@ -502,372 +1393,548 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.16796875" customWidth="true"/>
-    <col min="2" max="2" width="11.7109375" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="12.34765625" customWidth="true"/>
-    <col min="7" max="7" width="8.16796875" customWidth="true"/>
-    <col min="8" max="8" width="9.44140625" customWidth="true"/>
-    <col min="9" max="9" width="8.7109375" customWidth="true"/>
-    <col min="10" max="10" width="8.44140625" customWidth="true"/>
-    <col min="11" max="11" width="11.7109375" customWidth="true"/>
-    <col min="13" max="13" width="11.7109375" customWidth="true"/>
-    <col min="15" max="15" width="7.16796875" customWidth="true"/>
-    <col min="16" max="16" width="8.62109375" customWidth="true"/>
-    <col min="4" max="4" width="12.34765625" customWidth="true"/>
-    <col min="5" max="5" width="12.34765625" customWidth="true"/>
-    <col min="6" max="6" width="12.34765625" customWidth="true"/>
-    <col min="12" max="12" width="11.7109375" customWidth="true"/>
-    <col min="14" max="14" width="10.7109375" customWidth="true"/>
+    <col min="1" max="1" width="5.140625" customWidth="true"/>
+    <col min="2" max="2" width="9.140625" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="12.42578125" customWidth="true"/>
+    <col min="7" max="7" width="8.7109375" customWidth="true"/>
+    <col min="8" max="8" width="10.140625" customWidth="true"/>
+    <col min="9" max="9" width="9.42578125" customWidth="true"/>
+    <col min="10" max="10" width="9" customWidth="true"/>
+    <col min="11" max="11" width="11.5703125" customWidth="true"/>
+    <col min="13" max="13" width="12.28515625" customWidth="true"/>
+    <col min="15" max="15" width="13.5703125" customWidth="true"/>
+    <col min="16" max="16" width="15" customWidth="true"/>
+    <col min="4" max="4" width="12.42578125" customWidth="true"/>
+    <col min="5" max="5" width="12.42578125" customWidth="true"/>
+    <col min="6" max="6" width="12.42578125" customWidth="true"/>
+    <col min="12" max="12" width="13" customWidth="true"/>
+    <col min="14" max="14" width="11.85546875" customWidth="true"/>
+    <col min="17" max="17" width="14.28515625" customWidth="true"/>
+    <col min="18" max="18" width="13.85546875" customWidth="true"/>
+    <col min="19" max="19" width="11.7109375" customWidth="true"/>
+    <col min="20" max="20" width="10.7109375" customWidth="true"/>
+    <col min="21" max="21" width="11.7109375" customWidth="true"/>
+    <col min="22" max="22" width="10.7109375" customWidth="true"/>
+    <col min="23" max="23" width="7.5703125" customWidth="true"/>
+    <col min="24" max="24" width="9.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>324</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>36</v>
+        <v>325</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>37</v>
+        <v>326</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>38</v>
+        <v>327</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>39</v>
+        <v>328</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>40</v>
+        <v>329</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>41</v>
+        <v>330</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>42</v>
+        <v>331</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>43</v>
+        <v>332</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>44</v>
+        <v>333</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>45</v>
+        <v>334</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>46</v>
+        <v>335</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>47</v>
+        <v>336</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>48</v>
+        <v>337</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>49</v>
+        <v>338</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>50</v>
+        <v>339</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>99.999999998151907</v>
+        <v>99.99999999517604</v>
       </c>
       <c r="B2" s="0">
-        <v>1000000.0000000008</v>
+        <v>10000.000000000005</v>
       </c>
       <c r="C2" s="0">
-        <v>-7.5118606610455041</v>
+        <v>-8.5018220610823274</v>
       </c>
       <c r="D2" s="0">
-        <v>-7.52091268779711</v>
+        <v>-8.5018863549781614</v>
       </c>
       <c r="E2" s="0">
-        <v>-7.5101307468924752</v>
+        <v>-8.5018220503855488</v>
       </c>
       <c r="F2" s="0">
-        <v>-7.5115525143231654</v>
+        <v>-8.5018220504532636</v>
       </c>
       <c r="G2" s="0">
-        <v>121618</v>
+        <v>26180</v>
       </c>
       <c r="H2" s="0">
-        <v>14821</v>
+        <v>5214</v>
       </c>
       <c r="I2" s="0">
-        <v>375600</v>
+        <v>66991</v>
       </c>
       <c r="J2" s="0">
-        <v>7110</v>
+        <v>1081</v>
       </c>
       <c r="K2" s="0">
-        <v>512.31850229999998</v>
+        <v>65455</v>
       </c>
       <c r="L2" s="0">
-        <v>92.134071500000005</v>
+        <v>20848</v>
       </c>
       <c r="M2" s="0">
-        <v>1200.0024409</v>
+        <v>71087</v>
       </c>
       <c r="N2" s="0">
-        <v>28.6171939</v>
+        <v>1081</v>
       </c>
       <c r="O2" s="0">
+        <v>13091</v>
+      </c>
+      <c r="P2" s="0">
+        <v>15635</v>
+      </c>
+      <c r="Q2" s="0">
+        <v>66991</v>
+      </c>
+      <c r="R2" s="0">
+        <v>2127</v>
+      </c>
+      <c r="S2" s="0">
+        <v>91.668795200000005</v>
+      </c>
+      <c r="T2" s="0">
+        <v>27.308496300000002</v>
+      </c>
+      <c r="U2" s="0">
+        <v>110.8614257</v>
+      </c>
+      <c r="V2" s="0">
+        <v>3.2477933999999999</v>
+      </c>
+      <c r="W2" s="0">
         <v>9.9999999999999995e-07</v>
       </c>
-      <c r="P2" s="0" t="s">
-        <v>51</v>
+      <c r="X2" s="0" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>999.99999998416752</v>
+        <v>100.00000000001545</v>
       </c>
       <c r="B3" s="0">
-        <v>10000000</v>
+        <v>99999.999999935273</v>
       </c>
       <c r="C3" s="0">
-        <v>-75.118606610455046</v>
+        <v>-7.6040844172206485</v>
       </c>
       <c r="D3" s="0">
-        <v>-75.211016239359864</v>
+        <v>-7.605965997268906</v>
       </c>
       <c r="E3" s="0">
-        <v>-75.101516152466402</v>
+        <v>-7.6040824492821617</v>
       </c>
       <c r="F3" s="0">
-        <v>-75.115852522396793</v>
+        <v>-7.6040824603421768</v>
       </c>
       <c r="G3" s="0">
-        <v>121618</v>
+        <v>75680</v>
       </c>
       <c r="H3" s="0">
-        <v>14825</v>
+        <v>11081</v>
       </c>
       <c r="I3" s="0">
-        <v>379446</v>
+        <v>388313</v>
       </c>
       <c r="J3" s="0">
-        <v>10142</v>
+        <v>3343</v>
       </c>
       <c r="K3" s="0">
-        <v>515.77433689999998</v>
+        <v>189205</v>
       </c>
       <c r="L3" s="0">
-        <v>93.661196399999994</v>
+        <v>44316</v>
       </c>
       <c r="M3" s="0">
-        <v>1200.0062187999999</v>
+        <v>406024</v>
       </c>
       <c r="N3" s="0">
-        <v>40.084657900000003</v>
+        <v>3343</v>
       </c>
       <c r="O3" s="0">
+        <v>37841</v>
+      </c>
+      <c r="P3" s="0">
+        <v>33236</v>
+      </c>
+      <c r="Q3" s="0">
+        <v>388313</v>
+      </c>
+      <c r="R3" s="0">
+        <v>6655</v>
+      </c>
+      <c r="S3" s="0">
+        <v>261.81094089999999</v>
+      </c>
+      <c r="T3" s="0">
+        <v>58.121049800000002</v>
+      </c>
+      <c r="U3" s="0">
+        <v>652.03520470000001</v>
+      </c>
+      <c r="V3" s="0">
+        <v>9.9469472000000003</v>
+      </c>
+      <c r="W3" s="0">
         <v>9.9999999999999995e-07</v>
       </c>
-      <c r="P3" s="0" t="s">
-        <v>51</v>
+      <c r="X3" s="0" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>99.999999999170242</v>
+        <v>99.99999999825377</v>
       </c>
       <c r="B4" s="0">
-        <v>9999999.9990916178</v>
+        <v>1000000.0000000003</v>
       </c>
       <c r="C4" s="0">
-        <v>-7.4988601076838552</v>
+        <v>-7.5118606610451444</v>
       </c>
       <c r="D4" s="0">
-        <v>-5.5992913022744695</v>
+        <v>-7.5209126878658923</v>
       </c>
       <c r="E4" s="0">
-        <v>-7.456839633913436</v>
+        <v>-7.5106512797209994</v>
       </c>
       <c r="F4" s="0">
-        <v>-7.458520253104405</v>
+        <v>-7.5115525143231645</v>
       </c>
       <c r="G4" s="0">
-        <v>130302</v>
+        <v>121618</v>
       </c>
       <c r="H4" s="0">
-        <v>16582</v>
+        <v>14821</v>
       </c>
       <c r="I4" s="0">
-        <v>132227</v>
+        <v>701621</v>
       </c>
       <c r="J4" s="0">
-        <v>11893</v>
+        <v>7110</v>
       </c>
       <c r="K4" s="0">
-        <v>550.31302019999998</v>
+        <v>304050</v>
       </c>
       <c r="L4" s="0">
-        <v>104.7295883</v>
+        <v>59276</v>
       </c>
       <c r="M4" s="0">
-        <v>346.84264990000003</v>
+        <v>763507</v>
       </c>
       <c r="N4" s="0">
-        <v>47.024495899999998</v>
+        <v>7110</v>
       </c>
       <c r="O4" s="0">
+        <v>60810</v>
+      </c>
+      <c r="P4" s="0">
+        <v>44456</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>701621</v>
+      </c>
+      <c r="R4" s="0">
+        <v>14193</v>
+      </c>
+      <c r="S4" s="0">
+        <v>426.5035633</v>
+      </c>
+      <c r="T4" s="0">
+        <v>79.430768900000004</v>
+      </c>
+      <c r="U4" s="0">
+        <v>1200.0096814000001</v>
+      </c>
+      <c r="V4" s="0">
+        <v>21.161951200000001</v>
+      </c>
+      <c r="W4" s="0">
         <v>9.9999999999999995e-07</v>
       </c>
-      <c r="P4" s="0" t="s">
-        <v>51</v>
+      <c r="X4" s="0" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>10.000000000698492</v>
+        <v>999.99999998137355</v>
       </c>
       <c r="B5" s="0">
-        <v>9999999.9999999963</v>
+        <v>10000000.000000004</v>
       </c>
       <c r="C5" s="0">
-        <v>-0.74877875924638793</v>
+        <v>-75.1186066104475</v>
       </c>
       <c r="D5" s="0">
-        <v>0.69724256207684965</v>
+        <v>-75.211016239757214</v>
       </c>
       <c r="E5" s="0">
-        <v>-0.66132844733308338</v>
+        <v>-75.106325142222744</v>
       </c>
       <c r="F5" s="0">
-        <v>-0.68106492539102848</v>
+        <v>-75.115852522394704</v>
       </c>
       <c r="G5" s="0">
-        <v>230428</v>
+        <v>121618</v>
       </c>
       <c r="H5" s="0">
-        <v>35410</v>
+        <v>14825</v>
       </c>
       <c r="I5" s="0">
-        <v>43961</v>
+        <v>694397</v>
       </c>
       <c r="J5" s="0">
-        <v>20375</v>
+        <v>10142</v>
       </c>
       <c r="K5" s="0">
-        <v>994.06765700000005</v>
+        <v>304050</v>
       </c>
       <c r="L5" s="0">
-        <v>225.58642130000001</v>
+        <v>59292</v>
       </c>
       <c r="M5" s="0">
-        <v>116.73129950000001</v>
+        <v>756283</v>
       </c>
       <c r="N5" s="0">
-        <v>81.480997400000007</v>
+        <v>10142</v>
       </c>
       <c r="O5" s="0">
+        <v>60810</v>
+      </c>
+      <c r="P5" s="0">
+        <v>44468</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>694397</v>
+      </c>
+      <c r="R5" s="0">
+        <v>20258</v>
+      </c>
+      <c r="S5" s="0">
+        <v>433.8667868</v>
+      </c>
+      <c r="T5" s="0">
+        <v>81.445808999999997</v>
+      </c>
+      <c r="U5" s="0">
+        <v>1200.0027602</v>
+      </c>
+      <c r="V5" s="0">
+        <v>29.6895588</v>
+      </c>
+      <c r="W5" s="0">
         <v>9.9999999999999995e-07</v>
       </c>
-      <c r="P5" s="0" t="s">
-        <v>51</v>
+      <c r="X5" s="0" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>99.999999999170242</v>
+      <c r="A6" s="0">
+        <v>100.00000000143278</v>
       </c>
       <c r="B6" s="1">
-        <v>9999999.9990916178</v>
-      </c>
-      <c r="C6">
-        <v>-7.4988601076838552</v>
-      </c>
-      <c r="D6">
-        <v>-5.5992913022744695</v>
-      </c>
-      <c r="E6">
-        <v>-7.5020552480901657</v>
-      </c>
-      <c r="F6">
-        <v>-7.458520253104405</v>
-      </c>
-      <c r="G6">
+        <v>9999999.9992698189</v>
+      </c>
+      <c r="C6" s="0">
+        <v>-7.498860107817471</v>
+      </c>
+      <c r="D6" s="0">
+        <v>-5.5992912724044928</v>
+      </c>
+      <c r="E6" s="0">
+        <v>-7.4568396340436953</v>
+      </c>
+      <c r="F6" s="0">
+        <v>-7.4585202532400423</v>
+      </c>
+      <c r="G6" s="0">
         <v>130302</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>16582</v>
       </c>
-      <c r="I6">
-        <v>32743</v>
-      </c>
-      <c r="J6">
+      <c r="I6" s="0">
+        <v>132486</v>
+      </c>
+      <c r="J6" s="0">
         <v>11893</v>
       </c>
-      <c r="K6">
-        <v>611.52229339999997</v>
-      </c>
-      <c r="L6">
-        <v>114.7723979</v>
-      </c>
-      <c r="M6">
-        <v>92.425136199999997</v>
-      </c>
-      <c r="N6">
-        <v>50.775841</v>
-      </c>
-      <c r="O6">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="P6" t="s">
-        <v>17</v>
+      <c r="K6" s="0">
+        <v>325760</v>
+      </c>
+      <c r="L6" s="0">
+        <v>66320</v>
+      </c>
+      <c r="M6" s="0">
+        <v>264195</v>
+      </c>
+      <c r="N6" s="0">
+        <v>11893</v>
+      </c>
+      <c r="O6" s="0">
+        <v>65152</v>
+      </c>
+      <c r="P6" s="0">
+        <v>49739</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>132486</v>
+      </c>
+      <c r="R6" s="0">
+        <v>23760</v>
+      </c>
+      <c r="S6" s="0">
+        <v>454.35140949999999</v>
+      </c>
+      <c r="T6" s="0">
+        <v>86.083193300000005</v>
+      </c>
+      <c r="U6" s="0">
+        <v>248.52831130000001</v>
+      </c>
+      <c r="V6" s="0">
+        <v>34.178289200000002</v>
+      </c>
+      <c r="W6" s="0">
+        <v>9.9999999999999995e-07</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>10.000000000698492</v>
-      </c>
-      <c r="B7">
-        <v>9999999.9999999963</v>
-      </c>
-      <c r="C7">
-        <v>-0.74877875924638793</v>
-      </c>
-      <c r="D7">
-        <v>0.69724256207684965</v>
-      </c>
-      <c r="E7">
-        <v>-0.71090728929024405</v>
-      </c>
-      <c r="F7">
-        <v>-0.68106492539102848</v>
-      </c>
-      <c r="G7">
+      <c r="A7" s="0">
+        <v>10.000000001164153</v>
+      </c>
+      <c r="B7" s="0">
+        <v>9999999.9999999944</v>
+      </c>
+      <c r="C7" s="0">
+        <v>-0.74877875918500492</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1.2784488323982781</v>
+      </c>
+      <c r="E7" s="0">
+        <v>-0.66132844726916096</v>
+      </c>
+      <c r="F7" s="0">
+        <v>-0.68106492533591401</v>
+      </c>
+      <c r="G7" s="0">
         <v>230428</v>
       </c>
-      <c r="H7">
-        <v>35410</v>
-      </c>
-      <c r="I7">
-        <v>26509</v>
-      </c>
-      <c r="J7">
+      <c r="H7" s="0">
+        <v>35960</v>
+      </c>
+      <c r="I7" s="0">
+        <v>43985</v>
+      </c>
+      <c r="J7" s="0">
         <v>20375</v>
       </c>
-      <c r="K7">
-        <v>1074.6186835000001</v>
-      </c>
-      <c r="L7">
-        <v>241.800633</v>
-      </c>
-      <c r="M7">
-        <v>73.434905499999999</v>
-      </c>
-      <c r="N7">
-        <v>85.397531200000003</v>
-      </c>
-      <c r="O7">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="P7" t="s">
-        <v>17</v>
+      <c r="K7" s="0">
+        <v>576075</v>
+      </c>
+      <c r="L7" s="0">
+        <v>143832</v>
+      </c>
+      <c r="M7" s="0">
+        <v>87898</v>
+      </c>
+      <c r="N7" s="0">
+        <v>20375</v>
+      </c>
+      <c r="O7" s="0">
+        <v>115215</v>
+      </c>
+      <c r="P7" s="0">
+        <v>107873</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>43985</v>
+      </c>
+      <c r="R7" s="0">
+        <v>40724</v>
+      </c>
+      <c r="S7" s="0">
+        <v>793.68993209999996</v>
+      </c>
+      <c r="T7" s="0">
+        <v>188.34675039999999</v>
+      </c>
+      <c r="U7" s="0">
+        <v>83.0386515</v>
+      </c>
+      <c r="V7" s="0">
+        <v>58.216832500000002</v>
+      </c>
+      <c r="W7" s="0">
+        <v>9.9999999999999995e-07</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>